<commit_message>
modified sql tables, added documents for dev
</commit_message>
<xml_diff>
--- a/Web_final/presentation/req.xlsx
+++ b/Web_final/presentation/req.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18315" windowHeight="11670" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18315" windowHeight="11670" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="req" sheetId="2" r:id="rId1"/>
     <sheet name="spec" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="요구사항 분석" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="190">
   <si>
     <t>테이블정의서</t>
     <phoneticPr fontId="5" type="noConversion"/>
@@ -506,6 +506,277 @@
   </si>
   <si>
     <t>계약여부</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>우선순위</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>요구사항명</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>세부항목</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>내용</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>버전명</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>개발도구</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원가입</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>매물 등록</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>매물 검색</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>댓글 작성</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그인</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>마이페이지</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>이메일 인증</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>JS</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>닉네임 확인</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>이미 사용하고 있는 닉네임인지 확인</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>DB</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이디로 실제 존재하는 이메일인지 확인을 위한 이메일 인증</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>이메일 확인</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>이미 등록된 이메일인지 확인</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>공인중개사 번호 인증</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>비밀번호 유효성 검사</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>8 ~ 20 글자 및 특수문자 1개 이상 포함</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>매물 주소 입력</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>유효성 검사</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>사용자 위치 기반 검색</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>검색어로 검색</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>매물 상세보기</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>매물 사진 업로드</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>공인중개사 번호 형식에 맞는 번호인지 확인(xxxxx-xxxx-xxxxx)
+미입력시 일반 사용자로 가입</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>사용자가 입력한 검색어가 주소에 포함된 
+매물들을 출력</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>사용자 동의 후 위치 정보를 받아서 해당 
+위치 정보와 가까운 매물들을 출력</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>실제 존재하는 주소인지 지도 API를 이용하여 입력</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>사용자가 업로드하는 파일의 확장명을 이미지 파일로만 제한하여 검사 후 서버에 업로드</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>모든 검사 수행 후 입력 정보를 서버에 등록</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>검색 결과 페이지로 출력</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>검색 결과 출력되는 매물들을 페이지 단위로 출력</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>매물 상세화면 이동</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>검색 결과 표시되는 매물들마다 각각의 영역 선택시 상세화면으로 이동</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>HTML</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>상세정보 출력</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>매물의 주소, 등록한 사람, 매물 사진, 태그 출력</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>근처 편의시설 표시</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>현재 매물에서 일정 범위 내 편의시설을 지도에 표시</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>v2.0</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이디 및 비밀번호 확인</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>DB에 저장된 아이디, 비밀번호와 일치여부 확인</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>등록한 매물 확인/수정/삭제</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>작성한 리뷰 확인/수정/삭제</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>현재 로그인한 유저가 등록한 매물 확인, 정보 수정 및 매물 삭제</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>기존 작성된 리뷰에 댓글 작성</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>사용자가 저장한 댓글 내용을 저장</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>작성한 리뷰를 저장</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>보증금 , 월세 입력 확인</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>작성한 댓글 확인/삭제</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>현재 로그인한 유저가 작성한 리뷰 확인, 수정 및 삭제</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>현재 로그인한 유저가 작성한 댓글 확인 및 삭제</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>근처 동네 평가 보기</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>동네 리뷰 작성</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>동네 주소 입력</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>동네 평가 보기 버튼을 누르면 해당 매물이 속한 동네에 대한 리뷰 리스트 출력</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>현재 매물을 내 찜 목록에 추가</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>찜하기</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>찜 매물 확인/삭제</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>현재 로그인한 유저가 찜한 매물 확인 및 삭제</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>v1.0</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>작성한 리뷰 저장</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -569,7 +840,7 @@
       <charset val="129"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -582,8 +853,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="27">
+  <borders count="41">
     <border>
       <left/>
       <right/>
@@ -929,6 +1206,206 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -936,151 +1413,241 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="36" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1379,8 +1946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1391,24 +1958,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="17" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="20" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1416,7 +1983,7 @@
       <c r="A3" t="s">
         <v>68</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="21" t="s">
         <v>24</v>
       </c>
       <c r="C3" t="s">
@@ -1424,7 +1991,7 @@
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="21" t="s">
         <v>25</v>
       </c>
       <c r="C4" t="s">
@@ -1432,7 +1999,7 @@
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="21" t="s">
         <v>28</v>
       </c>
       <c r="C5" t="s">
@@ -1440,45 +2007,45 @@
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="37" t="s">
+      <c r="C6" s="22" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="38" t="s">
+      <c r="A7" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="38" t="s">
+      <c r="C7" s="23" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="38" t="s">
+      <c r="C8" s="23" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="38" t="s">
+      <c r="C9" s="23" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="21" t="s">
         <v>34</v>
       </c>
       <c r="C10" t="s">
@@ -1486,12 +2053,12 @@
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="21" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="21" t="s">
         <v>17</v>
       </c>
       <c r="C12" t="s">
@@ -1499,7 +2066,7 @@
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="B13" s="36" t="s">
+      <c r="B13" s="21" t="s">
         <v>122</v>
       </c>
       <c r="C13" t="s">
@@ -1507,13 +2074,13 @@
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="37" t="s">
+      <c r="A14" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="34" t="s">
+      <c r="B14" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="37" t="s">
+      <c r="C14" s="22" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1521,29 +2088,29 @@
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="36" t="s">
+      <c r="B15" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="38" t="s">
+      <c r="C15" s="23" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="37" t="s">
+      <c r="A16" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="B16" s="34" t="s">
+      <c r="B16" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="37" t="s">
+      <c r="C16" s="22" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="38" t="s">
+      <c r="A17" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="B17" s="36" t="s">
+      <c r="B17" s="21" t="s">
         <v>43</v>
       </c>
       <c r="C17" t="s">
@@ -1551,7 +2118,7 @@
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="B18" s="36" t="s">
+      <c r="B18" s="21" t="s">
         <v>44</v>
       </c>
       <c r="C18" t="s">
@@ -1559,7 +2126,7 @@
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="B19" s="36" t="s">
+      <c r="B19" s="21" t="s">
         <v>45</v>
       </c>
       <c r="C19" t="s">
@@ -1567,21 +2134,21 @@
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="37" t="s">
+      <c r="A20" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="34" t="s">
+      <c r="B20" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="37" t="s">
+      <c r="C20" s="22" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="38" t="s">
+      <c r="A21" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="B21" s="36" t="s">
+      <c r="B21" s="21" t="s">
         <v>51</v>
       </c>
       <c r="C21" t="s">
@@ -1589,21 +2156,21 @@
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="37" t="s">
+      <c r="A22" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="34" t="s">
+      <c r="B22" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="C22" s="37" t="s">
+      <c r="C22" s="22" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="38" t="s">
+      <c r="A23" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="B23" s="36" t="s">
+      <c r="B23" s="21" t="s">
         <v>52</v>
       </c>
       <c r="C23" t="s">
@@ -1611,7 +2178,7 @@
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="B24" s="36" t="s">
+      <c r="B24" s="21" t="s">
         <v>55</v>
       </c>
       <c r="C24" t="s">
@@ -1619,7 +2186,7 @@
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="B25" s="36" t="s">
+      <c r="B25" s="21" t="s">
         <v>56</v>
       </c>
       <c r="C25" t="s">
@@ -1627,7 +2194,7 @@
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="B26" s="36" t="s">
+      <c r="B26" s="21" t="s">
         <v>18</v>
       </c>
       <c r="C26" t="s">
@@ -1635,7 +2202,7 @@
       </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="B27" s="36" t="s">
+      <c r="B27" s="21" t="s">
         <v>57</v>
       </c>
       <c r="C27" t="s">
@@ -1643,7 +2210,7 @@
       </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="B28" s="36" t="s">
+      <c r="B28" s="21" t="s">
         <v>59</v>
       </c>
       <c r="C28" t="s">
@@ -1651,13 +2218,13 @@
       </c>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="37" t="s">
+      <c r="A29" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="B29" s="34" t="s">
+      <c r="B29" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="C29" s="37" t="s">
+      <c r="C29" s="22" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1665,7 +2232,7 @@
       <c r="A30" t="s">
         <v>73</v>
       </c>
-      <c r="B30" s="36" t="s">
+      <c r="B30" s="21" t="s">
         <v>52</v>
       </c>
       <c r="C30" t="s">
@@ -1673,7 +2240,7 @@
       </c>
     </row>
     <row r="31" spans="1:3">
-      <c r="B31" s="36" t="s">
+      <c r="B31" s="21" t="s">
         <v>53</v>
       </c>
       <c r="C31" t="s">
@@ -1681,7 +2248,7 @@
       </c>
     </row>
     <row r="32" spans="1:3">
-      <c r="B32" s="36" t="s">
+      <c r="B32" s="21" t="s">
         <v>18</v>
       </c>
       <c r="C32" t="s">
@@ -1689,7 +2256,7 @@
       </c>
     </row>
     <row r="33" spans="1:3">
-      <c r="B33" s="36" t="s">
+      <c r="B33" s="21" t="s">
         <v>57</v>
       </c>
       <c r="C33" t="s">
@@ -1697,7 +2264,7 @@
       </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="B34" s="36" t="s">
+      <c r="B34" s="21" t="s">
         <v>61</v>
       </c>
       <c r="C34" t="s">
@@ -1705,13 +2272,13 @@
       </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="37" t="s">
+      <c r="A35" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="B35" s="34" t="s">
+      <c r="B35" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C35" s="37" t="s">
+      <c r="C35" s="22" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1719,10 +2286,10 @@
       <c r="A36" t="s">
         <v>74</v>
       </c>
-      <c r="B36" s="36" t="s">
+      <c r="B36" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="C36" s="38" t="s">
+      <c r="C36" s="23" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1736,7 +2303,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
@@ -1749,1033 +2316,1086 @@
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="3"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" s="3"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="3"/>
+      <c r="A2" s="2"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:15">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:15">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="5" t="s">
+      <c r="B4" s="39"/>
+      <c r="C4" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="7"/>
-      <c r="I4" s="4" t="s">
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="42"/>
+      <c r="I4" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="J4" s="4"/>
-      <c r="K4" s="5" t="s">
+      <c r="J4" s="39"/>
+      <c r="K4" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="7"/>
+      <c r="L4" s="41"/>
+      <c r="M4" s="41"/>
+      <c r="N4" s="41"/>
+      <c r="O4" s="42"/>
     </row>
     <row r="5" spans="1:15" ht="16.5" customHeight="1">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="43" t="s">
         <v>117</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="5" t="s">
+      <c r="B5" s="44"/>
+      <c r="C5" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="7"/>
-      <c r="I5" s="8" t="s">
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="42"/>
+      <c r="I5" s="43" t="s">
         <v>117</v>
       </c>
-      <c r="J5" s="9"/>
-      <c r="K5" s="5" t="s">
+      <c r="J5" s="44"/>
+      <c r="K5" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="7"/>
+      <c r="L5" s="41"/>
+      <c r="M5" s="41"/>
+      <c r="N5" s="41"/>
+      <c r="O5" s="42"/>
     </row>
     <row r="6" spans="1:15" ht="24.75" thickBot="1">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="11"/>
-      <c r="I6" s="10" t="s">
+      <c r="G6" s="36"/>
+      <c r="I6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="J6" s="10" t="s">
+      <c r="J6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="K6" s="10" t="s">
+      <c r="K6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="L6" s="10" t="s">
+      <c r="L6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="M6" s="10" t="s">
+      <c r="M6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="N6" s="11" t="s">
+      <c r="N6" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="O6" s="11"/>
+      <c r="O6" s="36"/>
     </row>
     <row r="7" spans="1:15" ht="17.25" thickTop="1">
-      <c r="A7" s="12">
+      <c r="A7" s="4">
         <v>1</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="15"/>
-      <c r="G7" s="16"/>
-      <c r="I7" s="12">
+      <c r="F7" s="37"/>
+      <c r="G7" s="38"/>
+      <c r="I7" s="4">
         <v>1</v>
       </c>
-      <c r="J7" s="13" t="s">
+      <c r="J7" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="K7" s="19" t="s">
+      <c r="K7" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="L7" s="19" t="s">
+      <c r="L7" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="M7" s="14" t="s">
+      <c r="M7" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="N7" s="15"/>
-      <c r="O7" s="16"/>
+      <c r="N7" s="37"/>
+      <c r="O7" s="38"/>
     </row>
     <row r="8" spans="1:15">
-      <c r="A8" s="17">
+      <c r="A8" s="7">
         <f>SUM(A7,1)</f>
         <v>2</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="19"/>
-      <c r="F8" s="20" t="s">
+      <c r="E8" s="9"/>
+      <c r="F8" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="G8" s="21"/>
-      <c r="I8" s="25">
+      <c r="G8" s="33"/>
+      <c r="I8" s="12">
         <f t="shared" ref="I8" si="0">SUM(I7,1)</f>
         <v>2</v>
       </c>
-      <c r="J8" s="26" t="s">
+      <c r="J8" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="K8" s="27" t="s">
+      <c r="K8" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="L8" s="27" t="s">
+      <c r="L8" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="M8" s="27"/>
-      <c r="N8" s="28"/>
-      <c r="O8" s="29"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="29"/>
+      <c r="O8" s="30"/>
     </row>
     <row r="9" spans="1:15">
-      <c r="A9" s="17">
+      <c r="A9" s="7">
         <f t="shared" ref="A9:A10" si="1">SUM(A8,1)</f>
         <v>3</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="19"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="21"/>
-      <c r="I9" s="43"/>
-      <c r="J9" s="44"/>
-      <c r="K9" s="43"/>
-      <c r="L9" s="43"/>
-      <c r="M9" s="43"/>
-      <c r="N9" s="45"/>
-      <c r="O9" s="45"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="33"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="24"/>
+      <c r="M9" s="24"/>
+      <c r="N9" s="31"/>
+      <c r="O9" s="31"/>
     </row>
     <row r="10" spans="1:15">
-      <c r="A10" s="17">
+      <c r="A10" s="7">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="20" t="s">
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="G10" s="21"/>
+      <c r="G10" s="33"/>
     </row>
     <row r="11" spans="1:15">
-      <c r="A11" s="22"/>
-      <c r="B11" s="23"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
+      <c r="A11" s="10"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="47"/>
+      <c r="G11" s="47"/>
     </row>
     <row r="12" spans="1:15">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="5" t="s">
+      <c r="B12" s="39"/>
+      <c r="C12" s="40" t="s">
         <v>69</v>
       </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="7"/>
-      <c r="I12" s="4" t="s">
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="42"/>
+      <c r="I12" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="J12" s="4"/>
-      <c r="K12" s="5" t="s">
+      <c r="J12" s="39"/>
+      <c r="K12" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="7"/>
+      <c r="L12" s="41"/>
+      <c r="M12" s="41"/>
+      <c r="N12" s="41"/>
+      <c r="O12" s="42"/>
     </row>
     <row r="13" spans="1:15" ht="16.5" customHeight="1">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="43" t="s">
         <v>117</v>
       </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="5" t="s">
+      <c r="B13" s="44"/>
+      <c r="C13" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="7"/>
-      <c r="I13" s="8" t="s">
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="42"/>
+      <c r="I13" s="43" t="s">
         <v>117</v>
       </c>
-      <c r="J13" s="9"/>
-      <c r="K13" s="5" t="s">
+      <c r="J13" s="44"/>
+      <c r="K13" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="L13" s="6"/>
-      <c r="M13" s="6"/>
-      <c r="N13" s="6"/>
-      <c r="O13" s="7"/>
+      <c r="L13" s="41"/>
+      <c r="M13" s="41"/>
+      <c r="N13" s="41"/>
+      <c r="O13" s="42"/>
     </row>
     <row r="14" spans="1:15" ht="24.75" thickBot="1">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F14" s="11" t="s">
+      <c r="F14" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="G14" s="11"/>
-      <c r="I14" s="10" t="s">
+      <c r="G14" s="36"/>
+      <c r="I14" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="J14" s="10" t="s">
+      <c r="J14" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="K14" s="10" t="s">
+      <c r="K14" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="L14" s="10" t="s">
+      <c r="L14" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="M14" s="10" t="s">
+      <c r="M14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="N14" s="11" t="s">
+      <c r="N14" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="O14" s="11"/>
+      <c r="O14" s="36"/>
     </row>
     <row r="15" spans="1:15" ht="17.25" thickTop="1">
-      <c r="A15" s="12">
+      <c r="A15" s="4">
         <v>1</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="14" t="s">
+      <c r="E15" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F15" s="15" t="s">
+      <c r="F15" s="37" t="s">
         <v>92</v>
       </c>
-      <c r="G15" s="16"/>
-      <c r="I15" s="12">
+      <c r="G15" s="38"/>
+      <c r="I15" s="4">
         <v>1</v>
       </c>
-      <c r="J15" s="13" t="s">
+      <c r="J15" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="K15" s="19" t="s">
+      <c r="K15" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="L15" s="19" t="s">
+      <c r="L15" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="M15" s="14" t="s">
+      <c r="M15" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="N15" s="15" t="s">
+      <c r="N15" s="37" t="s">
         <v>110</v>
       </c>
-      <c r="O15" s="16"/>
+      <c r="O15" s="38"/>
     </row>
     <row r="16" spans="1:15">
-      <c r="A16" s="12">
+      <c r="A16" s="4">
         <v>2</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="C16" s="19" t="s">
+      <c r="C16" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="D16" s="19" t="s">
+      <c r="D16" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E16" s="14" t="s">
+      <c r="E16" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F16" s="39"/>
-      <c r="G16" s="40"/>
-      <c r="I16" s="12">
+      <c r="F16" s="27"/>
+      <c r="G16" s="28"/>
+      <c r="I16" s="4">
         <v>2</v>
       </c>
-      <c r="J16" s="13" t="s">
+      <c r="J16" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="K16" s="19" t="s">
+      <c r="K16" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="L16" s="19" t="s">
+      <c r="L16" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="M16" s="14" t="s">
+      <c r="M16" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="N16" s="39"/>
-      <c r="O16" s="40"/>
+      <c r="N16" s="27"/>
+      <c r="O16" s="28"/>
     </row>
     <row r="17" spans="1:15">
-      <c r="A17" s="12">
+      <c r="A17" s="4">
         <v>3</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="C17" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="D17" s="19" t="s">
+      <c r="D17" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="E17" s="14"/>
-      <c r="F17" s="39"/>
-      <c r="G17" s="40"/>
-      <c r="I17" s="12">
+      <c r="E17" s="6"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="28"/>
+      <c r="I17" s="4">
         <v>3</v>
       </c>
-      <c r="J17" s="13" t="s">
+      <c r="J17" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="K17" s="19" t="s">
+      <c r="K17" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="L17" s="19" t="s">
+      <c r="L17" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="M17" s="14" t="s">
+      <c r="M17" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="N17" s="39"/>
-      <c r="O17" s="40"/>
+      <c r="N17" s="27"/>
+      <c r="O17" s="28"/>
     </row>
     <row r="18" spans="1:15">
-      <c r="A18" s="12">
+      <c r="A18" s="4">
         <v>4</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="C18" s="19" t="s">
+      <c r="C18" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D18" s="19" t="s">
+      <c r="D18" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E18" s="14"/>
-      <c r="F18" s="39" t="s">
+      <c r="E18" s="6"/>
+      <c r="F18" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="G18" s="40"/>
-      <c r="I18" s="12">
+      <c r="G18" s="28"/>
+      <c r="I18" s="4">
         <v>4</v>
       </c>
-      <c r="J18" s="13" t="s">
+      <c r="J18" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="K18" s="19" t="s">
+      <c r="K18" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="L18" s="19" t="s">
+      <c r="L18" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="M18" s="14"/>
-      <c r="N18" s="39"/>
-      <c r="O18" s="40"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="27"/>
+      <c r="O18" s="28"/>
     </row>
     <row r="19" spans="1:15">
-      <c r="A19" s="12">
+      <c r="A19" s="4">
         <v>5</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="C19" s="19" t="s">
+      <c r="C19" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="19" t="s">
+      <c r="D19" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E19" s="14"/>
-      <c r="F19" s="39" t="s">
+      <c r="E19" s="6"/>
+      <c r="F19" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="G19" s="40"/>
-      <c r="I19" s="12">
+      <c r="G19" s="28"/>
+      <c r="I19" s="4">
         <v>5</v>
       </c>
-      <c r="J19" s="13" t="s">
+      <c r="J19" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="K19" s="19" t="s">
+      <c r="K19" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="L19" s="19" t="s">
+      <c r="L19" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="M19" s="14"/>
-      <c r="N19" s="39"/>
-      <c r="O19" s="40"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="27"/>
+      <c r="O19" s="28"/>
     </row>
     <row r="20" spans="1:15">
-      <c r="A20" s="12">
+      <c r="A20" s="4">
         <v>6</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="C20" s="19" t="s">
+      <c r="C20" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="21"/>
-      <c r="I20" s="17">
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="33"/>
+      <c r="I20" s="7">
         <v>6</v>
       </c>
-      <c r="J20" s="18" t="s">
+      <c r="J20" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="K20" s="19" t="s">
+      <c r="K20" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="L20" s="19"/>
-      <c r="M20" s="19"/>
-      <c r="N20" s="20" t="s">
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="O20" s="21"/>
+      <c r="O20" s="33"/>
     </row>
     <row r="21" spans="1:15" ht="16.5" customHeight="1">
-      <c r="A21" s="12">
+      <c r="A21" s="4">
         <v>7</v>
       </c>
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="C21" s="19" t="s">
+      <c r="C21" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="20" t="s">
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="G21" s="21"/>
-      <c r="I21" s="25">
+      <c r="G21" s="33"/>
+      <c r="I21" s="12">
         <v>7</v>
       </c>
-      <c r="J21" s="26" t="s">
+      <c r="J21" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="K21" s="27" t="s">
+      <c r="K21" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="L21" s="27"/>
-      <c r="M21" s="27"/>
-      <c r="N21" s="28" t="s">
+      <c r="L21" s="14"/>
+      <c r="M21" s="14"/>
+      <c r="N21" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="O21" s="29"/>
+      <c r="O21" s="30"/>
     </row>
     <row r="22" spans="1:15" ht="32.25" customHeight="1">
-      <c r="A22" s="25">
+      <c r="A22" s="12">
         <v>8</v>
       </c>
-      <c r="B22" s="26" t="s">
+      <c r="B22" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="C22" s="27" t="s">
+      <c r="C22" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="D22" s="27" t="s">
+      <c r="D22" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E22" s="27"/>
-      <c r="F22" s="47" t="s">
+      <c r="E22" s="14"/>
+      <c r="F22" s="34" t="s">
         <v>120</v>
       </c>
-      <c r="G22" s="48"/>
-      <c r="I22" s="43"/>
-      <c r="J22" s="44"/>
-      <c r="K22" s="43"/>
-      <c r="L22" s="43"/>
-      <c r="M22" s="43"/>
-      <c r="N22" s="46"/>
-      <c r="O22" s="46"/>
+      <c r="G22" s="35"/>
+      <c r="I22" s="24"/>
+      <c r="J22" s="25"/>
+      <c r="K22" s="24"/>
+      <c r="L22" s="24"/>
+      <c r="M22" s="24"/>
+      <c r="N22" s="26"/>
+      <c r="O22" s="26"/>
     </row>
     <row r="24" spans="1:15">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="4"/>
-      <c r="C24" s="5" t="s">
+      <c r="B24" s="39"/>
+      <c r="C24" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="7"/>
-      <c r="I24" s="4" t="s">
+      <c r="D24" s="41"/>
+      <c r="E24" s="41"/>
+      <c r="F24" s="41"/>
+      <c r="G24" s="42"/>
+      <c r="I24" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="J24" s="4"/>
-      <c r="K24" s="5" t="s">
+      <c r="J24" s="39"/>
+      <c r="K24" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="L24" s="6"/>
-      <c r="M24" s="6"/>
-      <c r="N24" s="6"/>
-      <c r="O24" s="7"/>
+      <c r="L24" s="41"/>
+      <c r="M24" s="41"/>
+      <c r="N24" s="41"/>
+      <c r="O24" s="42"/>
     </row>
     <row r="25" spans="1:15" ht="16.5" customHeight="1">
-      <c r="A25" s="8" t="s">
+      <c r="A25" s="43" t="s">
         <v>117</v>
       </c>
-      <c r="B25" s="9"/>
-      <c r="C25" s="5" t="s">
+      <c r="B25" s="44"/>
+      <c r="C25" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="7"/>
-      <c r="I25" s="8" t="s">
+      <c r="D25" s="41"/>
+      <c r="E25" s="41"/>
+      <c r="F25" s="41"/>
+      <c r="G25" s="42"/>
+      <c r="I25" s="43" t="s">
         <v>117</v>
       </c>
-      <c r="J25" s="9"/>
-      <c r="K25" s="5" t="s">
+      <c r="J25" s="44"/>
+      <c r="K25" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="L25" s="6"/>
-      <c r="M25" s="6"/>
-      <c r="N25" s="6"/>
-      <c r="O25" s="7"/>
+      <c r="L25" s="41"/>
+      <c r="M25" s="41"/>
+      <c r="N25" s="41"/>
+      <c r="O25" s="42"/>
     </row>
     <row r="26" spans="1:15" ht="24.75" thickBot="1">
-      <c r="A26" s="10" t="s">
+      <c r="A26" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C26" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D26" s="10" t="s">
+      <c r="D26" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E26" s="10" t="s">
+      <c r="E26" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F26" s="11" t="s">
+      <c r="F26" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="G26" s="11"/>
-      <c r="I26" s="10" t="s">
+      <c r="G26" s="36"/>
+      <c r="I26" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="J26" s="10" t="s">
+      <c r="J26" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="K26" s="10" t="s">
+      <c r="K26" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="L26" s="10" t="s">
+      <c r="L26" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="M26" s="10" t="s">
+      <c r="M26" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="N26" s="11" t="s">
+      <c r="N26" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="O26" s="11"/>
+      <c r="O26" s="36"/>
     </row>
     <row r="27" spans="1:15" ht="17.25" thickTop="1">
-      <c r="A27" s="12">
+      <c r="A27" s="4">
         <v>1</v>
       </c>
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="C27" s="19" t="s">
+      <c r="C27" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D27" s="19" t="s">
+      <c r="D27" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E27" s="14" t="s">
+      <c r="E27" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F27" s="15"/>
-      <c r="G27" s="16"/>
-      <c r="I27" s="12">
+      <c r="F27" s="37"/>
+      <c r="G27" s="38"/>
+      <c r="I27" s="4">
         <v>1</v>
       </c>
-      <c r="J27" s="13" t="s">
+      <c r="J27" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="K27" s="19" t="s">
+      <c r="K27" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="L27" s="19" t="s">
+      <c r="L27" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="M27" s="14" t="s">
+      <c r="M27" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="N27" s="15" t="s">
+      <c r="N27" s="37" t="s">
         <v>115</v>
       </c>
-      <c r="O27" s="16"/>
+      <c r="O27" s="38"/>
     </row>
     <row r="28" spans="1:15">
-      <c r="A28" s="25">
+      <c r="A28" s="12">
         <v>2</v>
       </c>
-      <c r="B28" s="26" t="s">
+      <c r="B28" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="C28" s="27" t="s">
+      <c r="C28" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="D28" s="27" t="s">
+      <c r="D28" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E28" s="27"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="29"/>
-      <c r="I28" s="12">
+      <c r="E28" s="14"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="30"/>
+      <c r="I28" s="4">
         <v>2</v>
       </c>
-      <c r="J28" s="13" t="s">
+      <c r="J28" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="K28" s="19" t="s">
+      <c r="K28" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="L28" s="19" t="s">
+      <c r="L28" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="M28" s="14" t="s">
+      <c r="M28" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="N28" s="39"/>
-      <c r="O28" s="40"/>
+      <c r="N28" s="27"/>
+      <c r="O28" s="28"/>
     </row>
     <row r="29" spans="1:15">
-      <c r="I29" s="12">
+      <c r="I29" s="4">
         <v>3</v>
       </c>
-      <c r="J29" s="13" t="s">
+      <c r="J29" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="K29" s="19" t="s">
+      <c r="K29" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="L29" s="19" t="s">
+      <c r="L29" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="M29" s="14" t="s">
+      <c r="M29" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="N29" s="39"/>
-      <c r="O29" s="40"/>
+      <c r="N29" s="27"/>
+      <c r="O29" s="28"/>
     </row>
     <row r="30" spans="1:15">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B30" s="4"/>
-      <c r="C30" s="5" t="s">
+      <c r="B30" s="39"/>
+      <c r="C30" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="7"/>
-      <c r="I30" s="12">
+      <c r="D30" s="41"/>
+      <c r="E30" s="41"/>
+      <c r="F30" s="41"/>
+      <c r="G30" s="42"/>
+      <c r="I30" s="4">
         <v>4</v>
       </c>
-      <c r="J30" s="13" t="s">
+      <c r="J30" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="K30" s="19" t="s">
+      <c r="K30" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="L30" s="19" t="s">
+      <c r="L30" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="M30" s="14"/>
-      <c r="N30" s="39"/>
-      <c r="O30" s="40"/>
+      <c r="M30" s="6"/>
+      <c r="N30" s="27"/>
+      <c r="O30" s="28"/>
     </row>
     <row r="31" spans="1:15" ht="16.5" customHeight="1">
-      <c r="A31" s="8" t="s">
+      <c r="A31" s="43" t="s">
         <v>117</v>
       </c>
-      <c r="B31" s="9"/>
-      <c r="C31" s="5" t="s">
+      <c r="B31" s="44"/>
+      <c r="C31" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="7"/>
-      <c r="I31" s="12">
+      <c r="D31" s="41"/>
+      <c r="E31" s="41"/>
+      <c r="F31" s="41"/>
+      <c r="G31" s="42"/>
+      <c r="I31" s="4">
         <v>5</v>
       </c>
-      <c r="J31" s="18" t="s">
+      <c r="J31" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="K31" s="19" t="s">
+      <c r="K31" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="L31" s="19"/>
-      <c r="M31" s="19"/>
-      <c r="N31" s="20" t="s">
+      <c r="L31" s="9"/>
+      <c r="M31" s="9"/>
+      <c r="N31" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="O31" s="21"/>
+      <c r="O31" s="33"/>
     </row>
     <row r="32" spans="1:15" ht="24.75" thickBot="1">
-      <c r="A32" s="10" t="s">
+      <c r="A32" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B32" s="10" t="s">
+      <c r="B32" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C32" s="10" t="s">
+      <c r="C32" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D32" s="10" t="s">
+      <c r="D32" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E32" s="10" t="s">
+      <c r="E32" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F32" s="11" t="s">
+      <c r="F32" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="G32" s="11"/>
-      <c r="I32" s="25">
+      <c r="G32" s="36"/>
+      <c r="I32" s="12">
         <v>6</v>
       </c>
-      <c r="J32" s="26" t="s">
+      <c r="J32" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="K32" s="27" t="s">
+      <c r="K32" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="L32" s="27"/>
-      <c r="M32" s="27"/>
-      <c r="N32" s="28" t="s">
+      <c r="L32" s="14"/>
+      <c r="M32" s="14"/>
+      <c r="N32" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="O32" s="29"/>
+      <c r="O32" s="30"/>
     </row>
     <row r="33" spans="1:15" ht="17.25" thickTop="1">
-      <c r="A33" s="12">
+      <c r="A33" s="4">
         <v>1</v>
       </c>
-      <c r="B33" s="13" t="s">
+      <c r="B33" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="C33" s="19" t="s">
+      <c r="C33" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D33" s="19" t="s">
+      <c r="D33" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E33" s="14" t="s">
+      <c r="E33" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F33" s="15"/>
-      <c r="G33" s="16"/>
-      <c r="I33" s="43"/>
-      <c r="J33" s="44"/>
-      <c r="K33" s="43"/>
-      <c r="L33" s="43"/>
-      <c r="M33" s="43"/>
-      <c r="N33" s="45"/>
-      <c r="O33" s="45"/>
+      <c r="F33" s="37"/>
+      <c r="G33" s="38"/>
+      <c r="I33" s="24"/>
+      <c r="J33" s="25"/>
+      <c r="K33" s="24"/>
+      <c r="L33" s="24"/>
+      <c r="M33" s="24"/>
+      <c r="N33" s="31"/>
+      <c r="O33" s="31"/>
     </row>
     <row r="34" spans="1:15">
-      <c r="A34" s="12">
+      <c r="A34" s="4">
         <v>2</v>
       </c>
-      <c r="B34" s="13" t="s">
+      <c r="B34" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C34" s="19" t="s">
+      <c r="C34" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="D34" s="19"/>
-      <c r="E34" s="14"/>
-      <c r="F34" s="39" t="s">
+      <c r="D34" s="9"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="G34" s="40"/>
-      <c r="I34" s="4" t="s">
+      <c r="G34" s="28"/>
+      <c r="I34" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="J34" s="4"/>
-      <c r="K34" s="5" t="s">
+      <c r="J34" s="39"/>
+      <c r="K34" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="L34" s="6"/>
-      <c r="M34" s="6"/>
-      <c r="N34" s="6"/>
-      <c r="O34" s="7"/>
+      <c r="L34" s="41"/>
+      <c r="M34" s="41"/>
+      <c r="N34" s="41"/>
+      <c r="O34" s="42"/>
     </row>
     <row r="35" spans="1:15">
-      <c r="A35" s="17">
+      <c r="A35" s="7">
         <v>3</v>
       </c>
-      <c r="B35" s="18" t="s">
+      <c r="B35" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="C35" s="19" t="s">
+      <c r="C35" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="D35" s="19"/>
-      <c r="E35" s="19"/>
-      <c r="F35" s="39" t="s">
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="G35" s="40"/>
-      <c r="I35" s="8" t="s">
+      <c r="G35" s="28"/>
+      <c r="I35" s="43" t="s">
         <v>116</v>
       </c>
-      <c r="J35" s="9"/>
-      <c r="K35" s="5" t="s">
+      <c r="J35" s="44"/>
+      <c r="K35" s="40" t="s">
         <v>118</v>
       </c>
-      <c r="L35" s="6"/>
-      <c r="M35" s="6"/>
-      <c r="N35" s="6"/>
-      <c r="O35" s="7"/>
+      <c r="L35" s="41"/>
+      <c r="M35" s="41"/>
+      <c r="N35" s="41"/>
+      <c r="O35" s="42"/>
     </row>
     <row r="36" spans="1:15" ht="24.75" thickBot="1">
-      <c r="A36" s="25">
+      <c r="A36" s="12">
         <v>4</v>
       </c>
-      <c r="B36" s="26" t="s">
+      <c r="B36" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="C36" s="27" t="s">
+      <c r="C36" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="D36" s="27"/>
-      <c r="E36" s="27"/>
-      <c r="F36" s="41" t="s">
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="G36" s="42"/>
-      <c r="I36" s="10" t="s">
+      <c r="G36" s="46"/>
+      <c r="I36" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="J36" s="10" t="s">
+      <c r="J36" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="K36" s="10" t="s">
+      <c r="K36" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="L36" s="10" t="s">
+      <c r="L36" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="M36" s="10" t="s">
+      <c r="M36" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="N36" s="11" t="s">
+      <c r="N36" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="O36" s="11"/>
+      <c r="O36" s="36"/>
     </row>
     <row r="37" spans="1:15" ht="17.25" thickTop="1">
-      <c r="I37" s="12">
+      <c r="I37" s="4">
         <v>1</v>
       </c>
-      <c r="J37" s="13" t="s">
+      <c r="J37" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="K37" s="19" t="s">
+      <c r="K37" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="L37" s="19" t="s">
+      <c r="L37" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="M37" s="14" t="s">
+      <c r="M37" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="N37" s="15"/>
-      <c r="O37" s="16"/>
+      <c r="N37" s="37"/>
+      <c r="O37" s="38"/>
     </row>
     <row r="38" spans="1:15">
-      <c r="I38" s="25">
+      <c r="I38" s="12">
         <v>2</v>
       </c>
-      <c r="J38" s="26" t="s">
+      <c r="J38" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="K38" s="27" t="s">
+      <c r="K38" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="L38" s="27" t="s">
+      <c r="L38" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="M38" s="27" t="s">
+      <c r="M38" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="N38" s="28"/>
-      <c r="O38" s="29"/>
+      <c r="N38" s="29"/>
+      <c r="O38" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="79">
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="N19:O19"/>
-    <mergeCell ref="N28:O28"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="B1:F2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="N37:O37"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="K4:O4"/>
+    <mergeCell ref="I35:J35"/>
+    <mergeCell ref="K35:O35"/>
+    <mergeCell ref="N36:O36"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:O5"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="K24:O24"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="K25:O25"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="K12:O12"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="K13:O13"/>
+    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="N15:O15"/>
     <mergeCell ref="N29:O29"/>
     <mergeCell ref="N38:O38"/>
     <mergeCell ref="F18:G18"/>
@@ -2792,64 +3412,11 @@
     <mergeCell ref="K34:O34"/>
     <mergeCell ref="N20:O20"/>
     <mergeCell ref="N21:O21"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="K24:O24"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="K25:O25"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="K12:O12"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="K13:O13"/>
-    <mergeCell ref="N14:O14"/>
-    <mergeCell ref="N15:O15"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:O5"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="N8:O8"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="K4:O4"/>
-    <mergeCell ref="I35:J35"/>
-    <mergeCell ref="K35:O35"/>
-    <mergeCell ref="N36:O36"/>
-    <mergeCell ref="N37:O37"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="B1:F2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="N28:O28"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2858,12 +3425,510 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="9" style="53"/>
+    <col min="2" max="2" width="15.5" customWidth="1"/>
+    <col min="3" max="3" width="26.5" customWidth="1"/>
+    <col min="4" max="4" width="38.75" style="51" customWidth="1"/>
+    <col min="5" max="5" width="10.625" customWidth="1"/>
+    <col min="6" max="6" width="12.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="55" t="s">
+        <v>123</v>
+      </c>
+      <c r="B1" s="56" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1" s="56" t="s">
+        <v>125</v>
+      </c>
+      <c r="D1" s="57" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1" s="56" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1" s="71" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="33">
+      <c r="A2" s="60">
+        <v>2</v>
+      </c>
+      <c r="B2" s="50" t="s">
+        <v>129</v>
+      </c>
+      <c r="C2" s="50" t="s">
+        <v>135</v>
+      </c>
+      <c r="D2" s="58" t="s">
+        <v>140</v>
+      </c>
+      <c r="E2" s="50" t="s">
+        <v>167</v>
+      </c>
+      <c r="F2" s="72" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="60">
+        <v>1</v>
+      </c>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50" t="s">
+        <v>141</v>
+      </c>
+      <c r="D3" s="58" t="s">
+        <v>142</v>
+      </c>
+      <c r="E3" s="50" t="s">
+        <v>188</v>
+      </c>
+      <c r="F3" s="72" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="60">
+        <v>1</v>
+      </c>
+      <c r="B4" s="50"/>
+      <c r="C4" s="50" t="s">
+        <v>137</v>
+      </c>
+      <c r="D4" s="58" t="s">
+        <v>138</v>
+      </c>
+      <c r="E4" s="50" t="s">
+        <v>188</v>
+      </c>
+      <c r="F4" s="72" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="49.5">
+      <c r="A5" s="60">
+        <v>1</v>
+      </c>
+      <c r="B5" s="50"/>
+      <c r="C5" s="50" t="s">
+        <v>143</v>
+      </c>
+      <c r="D5" s="58" t="s">
+        <v>152</v>
+      </c>
+      <c r="E5" s="50" t="s">
+        <v>188</v>
+      </c>
+      <c r="F5" s="72" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="52" customFormat="1" ht="17.25" thickBot="1">
+      <c r="A6" s="64">
+        <v>1</v>
+      </c>
+      <c r="B6" s="65"/>
+      <c r="C6" s="65" t="s">
+        <v>144</v>
+      </c>
+      <c r="D6" s="66" t="s">
+        <v>145</v>
+      </c>
+      <c r="E6" s="65" t="s">
+        <v>188</v>
+      </c>
+      <c r="F6" s="73" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="33.75" thickTop="1">
+      <c r="A7" s="61">
+        <v>2</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="C7" s="62" t="s">
+        <v>146</v>
+      </c>
+      <c r="D7" s="63" t="s">
+        <v>155</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="F7" s="74" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="60">
+        <v>1</v>
+      </c>
+      <c r="B8" s="50"/>
+      <c r="C8" s="59" t="s">
+        <v>147</v>
+      </c>
+      <c r="D8" s="58" t="s">
+        <v>176</v>
+      </c>
+      <c r="E8" s="50" t="s">
+        <v>188</v>
+      </c>
+      <c r="F8" s="75" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="33">
+      <c r="A9" s="60">
+        <v>1</v>
+      </c>
+      <c r="B9" s="50"/>
+      <c r="C9" s="59" t="s">
+        <v>151</v>
+      </c>
+      <c r="D9" s="58" t="s">
+        <v>156</v>
+      </c>
+      <c r="E9" s="50" t="s">
+        <v>188</v>
+      </c>
+      <c r="F9" s="72" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="52" customFormat="1" ht="17.25" thickBot="1">
+      <c r="A10" s="64">
+        <v>1</v>
+      </c>
+      <c r="B10" s="65"/>
+      <c r="C10" s="65" t="s">
+        <v>130</v>
+      </c>
+      <c r="D10" s="66" t="s">
+        <v>157</v>
+      </c>
+      <c r="E10" s="65" t="s">
+        <v>188</v>
+      </c>
+      <c r="F10" s="73" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="33.75" thickTop="1">
+      <c r="A11" s="61">
+        <v>2</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="D11" s="63" t="s">
+        <v>154</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="F11" s="74" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="33">
+      <c r="A12" s="60">
+        <v>1</v>
+      </c>
+      <c r="B12" s="50"/>
+      <c r="C12" s="50" t="s">
+        <v>149</v>
+      </c>
+      <c r="D12" s="58" t="s">
+        <v>153</v>
+      </c>
+      <c r="E12" s="50" t="s">
+        <v>188</v>
+      </c>
+      <c r="F12" s="75" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="52" customFormat="1" ht="33.75" thickBot="1">
+      <c r="A13" s="64">
+        <v>1</v>
+      </c>
+      <c r="B13" s="65"/>
+      <c r="C13" s="65" t="s">
+        <v>158</v>
+      </c>
+      <c r="D13" s="66" t="s">
+        <v>159</v>
+      </c>
+      <c r="E13" s="65" t="s">
+        <v>188</v>
+      </c>
+      <c r="F13" s="73" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="33.75" thickTop="1">
+      <c r="A14" s="61">
+        <v>1</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="C14" s="62" t="s">
+        <v>160</v>
+      </c>
+      <c r="D14" s="63" t="s">
+        <v>161</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="F14" s="76" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="33">
+      <c r="A15" s="60">
+        <v>1</v>
+      </c>
+      <c r="B15" s="50"/>
+      <c r="C15" s="59" t="s">
+        <v>163</v>
+      </c>
+      <c r="D15" s="58" t="s">
+        <v>164</v>
+      </c>
+      <c r="E15" s="50" t="s">
+        <v>188</v>
+      </c>
+      <c r="F15" s="72" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" s="49" customFormat="1" ht="33">
+      <c r="A16" s="60">
+        <v>2</v>
+      </c>
+      <c r="B16" s="50"/>
+      <c r="C16" s="59" t="s">
+        <v>165</v>
+      </c>
+      <c r="D16" s="58" t="s">
+        <v>166</v>
+      </c>
+      <c r="E16" s="50" t="s">
+        <v>167</v>
+      </c>
+      <c r="F16" s="72" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="49" customFormat="1">
+      <c r="A17" s="60">
+        <v>1</v>
+      </c>
+      <c r="B17" s="50"/>
+      <c r="C17" s="59" t="s">
+        <v>185</v>
+      </c>
+      <c r="D17" s="58" t="s">
+        <v>184</v>
+      </c>
+      <c r="E17" s="50" t="s">
+        <v>188</v>
+      </c>
+      <c r="F17" s="75" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="52" customFormat="1" ht="33.75" thickBot="1">
+      <c r="A18" s="64">
+        <v>2</v>
+      </c>
+      <c r="B18" s="65"/>
+      <c r="C18" s="67" t="s">
+        <v>180</v>
+      </c>
+      <c r="D18" s="66" t="s">
+        <v>183</v>
+      </c>
+      <c r="E18" s="65" t="s">
+        <v>167</v>
+      </c>
+      <c r="F18" s="73" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="54" customFormat="1" ht="34.5" thickTop="1" thickBot="1">
+      <c r="A19" s="68">
+        <v>1</v>
+      </c>
+      <c r="B19" s="69" t="s">
+        <v>133</v>
+      </c>
+      <c r="C19" s="69" t="s">
+        <v>168</v>
+      </c>
+      <c r="D19" s="70" t="s">
+        <v>169</v>
+      </c>
+      <c r="E19" s="69" t="s">
+        <v>188</v>
+      </c>
+      <c r="F19" s="77" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="33.75" thickTop="1">
+      <c r="A20" s="61">
+        <v>1</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>170</v>
+      </c>
+      <c r="D20" s="63" t="s">
+        <v>172</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="F20" s="76" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="33">
+      <c r="A21" s="60">
+        <v>1</v>
+      </c>
+      <c r="B21" s="50"/>
+      <c r="C21" s="50" t="s">
+        <v>171</v>
+      </c>
+      <c r="D21" s="58" t="s">
+        <v>178</v>
+      </c>
+      <c r="E21" s="50" t="s">
+        <v>188</v>
+      </c>
+      <c r="F21" s="72" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="60">
+        <v>1</v>
+      </c>
+      <c r="B22" s="50"/>
+      <c r="C22" s="50" t="s">
+        <v>186</v>
+      </c>
+      <c r="D22" s="58" t="s">
+        <v>187</v>
+      </c>
+      <c r="E22" s="50" t="s">
+        <v>188</v>
+      </c>
+      <c r="F22" s="72" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" s="52" customFormat="1" ht="33.75" thickBot="1">
+      <c r="A23" s="64">
+        <v>1</v>
+      </c>
+      <c r="B23" s="65"/>
+      <c r="C23" s="65" t="s">
+        <v>177</v>
+      </c>
+      <c r="D23" s="66" t="s">
+        <v>179</v>
+      </c>
+      <c r="E23" s="65" t="s">
+        <v>188</v>
+      </c>
+      <c r="F23" s="73" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="33.75" thickTop="1">
+      <c r="A24" s="61">
+        <v>2</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="C24" s="62" t="s">
+        <v>182</v>
+      </c>
+      <c r="D24" s="63" t="s">
+        <v>155</v>
+      </c>
+      <c r="E24" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="F24" s="74" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" s="52" customFormat="1" ht="17.25" thickBot="1">
+      <c r="A25" s="64">
+        <v>1</v>
+      </c>
+      <c r="B25" s="65"/>
+      <c r="C25" s="65" t="s">
+        <v>189</v>
+      </c>
+      <c r="D25" s="66" t="s">
+        <v>175</v>
+      </c>
+      <c r="E25" s="65" t="s">
+        <v>188</v>
+      </c>
+      <c r="F25" s="78" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" s="54" customFormat="1" ht="18" thickTop="1" thickBot="1">
+      <c r="A26" s="68">
+        <v>1</v>
+      </c>
+      <c r="B26" s="69" t="s">
+        <v>132</v>
+      </c>
+      <c r="C26" s="69" t="s">
+        <v>173</v>
+      </c>
+      <c r="D26" s="70" t="s">
+        <v>174</v>
+      </c>
+      <c r="E26" s="69" t="s">
+        <v>188</v>
+      </c>
+      <c r="F26" s="77" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="17.25" thickTop="1"/>
+  </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>